<commit_message>
Initial commit: Pipe Catalogue
</commit_message>
<xml_diff>
--- a/Pipe Catalogue.xlsx
+++ b/Pipe Catalogue.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Makroer &amp; Beregningsark\Beregningsark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2971BDB1-3C06-49CA-9770-47645CD403B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C4C4CF-ADFA-4EA8-AEC1-7DB423737EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{DAC88BDC-18A3-4C41-BAA6-C6E03CF8098A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DAC88BDC-18A3-4C41-BAA6-C6E03CF8098A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="26">
   <si>
     <t>Material</t>
   </si>
@@ -119,6 +119,24 @@
   <si>
     <t>B2</t>
   </si>
+  <si>
+    <t>Dybde</t>
+  </si>
+  <si>
+    <t>Thick_bot_1</t>
+  </si>
+  <si>
+    <t>Thick_bot_2</t>
+  </si>
+  <si>
+    <t>moh</t>
+  </si>
+  <si>
+    <t>Invert Level_1</t>
+  </si>
+  <si>
+    <t>Invert Level_2</t>
+  </si>
 </sst>
 </file>
 
@@ -171,7 +189,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -194,20 +212,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="1" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -231,16 +263,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>256761</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>381085</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>505324</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>172058</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -263,8 +295,52 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10248900" y="180975"/>
-          <a:ext cx="4762585" cy="2533650"/>
+          <a:off x="8622196" y="0"/>
+          <a:ext cx="3926041" cy="2077058"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>364435</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>132627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>260653</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>31056</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1619EF3-1D02-A009-8D8B-9F65F0B213D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8729870" y="2228127"/>
+          <a:ext cx="2347870" cy="2946429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -628,11 +704,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -656,13 +732,13 @@
       <c r="G2">
         <v>408</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="2">
-        <v>1200</v>
-      </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="1">
+        <v>1400</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -688,13 +764,13 @@
       <c r="G3">
         <v>544</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -718,14 +794,14 @@
       <c r="G4">
         <v>757</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="4" cm="1">
+      <c r="J4" s="3" cm="1">
         <f t="array" ref="J4">INDEX(Table1[Thick_side],MATCH(J2&amp;J3,Table1[Intern_dia]&amp;Table1[Material],0))</f>
-        <v>138</v>
-      </c>
-      <c r="K4" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -751,13 +827,13 @@
       <c r="G5">
         <v>879</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="2">
-        <v>1600</v>
-      </c>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="1">
+        <v>900</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -783,13 +859,13 @@
       <c r="G6">
         <v>1025</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="2"/>
+      <c r="J6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -813,14 +889,14 @@
       <c r="G7">
         <v>1171</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="4" cm="1">
+      <c r="J7" s="3" cm="1">
         <f t="array" ref="J7">INDEX(Table1[Thick_side],MATCH(J5&amp;J6,Table1[Intern_dia]&amp;Table1[Material],0))</f>
-        <v>19.25</v>
-      </c>
-      <c r="K7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -846,13 +922,13 @@
       <c r="G8">
         <v>1317</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="2">
-        <v>1000</v>
-      </c>
-      <c r="K8" s="2" t="s">
+      <c r="J8" s="1">
+        <v>500</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -878,14 +954,14 @@
       <c r="G9">
         <v>1464</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <f>J2/2+J4+J5/2+J7+J8</f>
-        <v>2557.25</v>
-      </c>
-      <c r="K9" s="3" t="s">
+        <v>1920</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1026,6 +1102,11 @@
       <c r="G15">
         <v>427.3</v>
       </c>
+      <c r="I15" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1049,8 +1130,17 @@
       <c r="G16">
         <v>475.8</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="1">
+        <v>800</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1072,8 +1162,15 @@
       <c r="G17">
         <v>530.29999999999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1095,8 +1192,18 @@
       <c r="G18">
         <v>633</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J18" s="3" cm="1">
+        <f t="array" ref="J18">INDEX(Table1[Thick_bot],MATCH(J16&amp;J17,Table1[Intern_dia]&amp;Table1[Material],0))</f>
+        <v>225</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1118,8 +1225,17 @@
       <c r="G19">
         <v>718.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1141,8 +1257,15 @@
       <c r="G20">
         <v>820.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1164,8 +1287,18 @@
       <c r="G21">
         <v>924</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="3" cm="1">
+        <f t="array" ref="J21">INDEX(Table1[Thick_side],MATCH(J19&amp;J20,Table1[Intern_dia]&amp;Table1[Material],0))</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1187,8 +1320,17 @@
       <c r="G22">
         <v>1026.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="1">
+        <v>200</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1210,8 +1352,18 @@
       <c r="G23">
         <v>1125.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="3">
+        <f>J18+J19+J21+J22</f>
+        <v>1425</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1233,8 +1385,17 @@
       <c r="G24">
         <v>1229</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="1">
+        <v>1.55</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1256,8 +1417,18 @@
       <c r="G25">
         <v>1331.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" s="6">
+        <f>J24-J23/1000</f>
+        <v>0.125</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1280,7 +1451,7 @@
         <v>1433.5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -1303,7 +1474,7 @@
         <v>1536.5</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1326,7 +1497,7 @@
         <v>1638.5</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -1349,7 +1520,7 @@
         <v>1739.5</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1372,7 +1543,7 @@
         <v>1841.5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -1395,7 +1566,7 @@
         <v>1944.5</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -2477,10 +2648,14 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="I1:K1"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Verdana"&amp;7&amp;K000000 Confidential</oddFooter>
+  </headerFooter>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>